<commit_message>
update int 64 pes configuration
</commit_message>
<xml_diff>
--- a/dtpu_configurations/only_integer16/100mhz/graph.xlsx
+++ b/dtpu_configurations/only_integer16/100mhz/graph.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8990FB7-3F52-4F88-8AB9-5613D8935655}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53117610-516D-4F71-8A93-B6FF70DE33DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="utilizaiton" sheetId="1" r:id="rId1"/>
     <sheet name="timing" sheetId="2" r:id="rId2"/>
     <sheet name="power" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
   <si>
     <t>Clocks</t>
   </si>
@@ -87,11 +97,17 @@
   <si>
     <t>BUFG</t>
   </si>
+  <si>
+    <t>PL dynamic</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,12 +150,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="18" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1501,1242 +1524,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:depthPercent val="100"/>
-      <c:rAngAx val="1"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:backWall>
-    <c:plotArea>
-      <c:layout/>
-      <c:bar3DChart>
-        <c:barDir val="col"/>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>power!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Clocks</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>power!$A$2:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7x7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8x8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10x10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>power!$B$2:$B$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.05</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-99F5-4827-9632-6E18FEE23E7A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>power!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Signals</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>power!$A$2:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7x7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8x8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10x10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>power!$C$2:$C$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.02</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-99F5-4827-9632-6E18FEE23E7A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>power!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Logic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>power!$A$2:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7x7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8x8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10x10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>power!$D$2:$D$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.01</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-99F5-4827-9632-6E18FEE23E7A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>power!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>BRAM</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>power!$A$2:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7x7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8x8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10x10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>power!$E$2:$E$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.01</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-99F5-4827-9632-6E18FEE23E7A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>power!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DSP</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>power!$A$2:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7x7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8x8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10x10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>power!$F$2:$F$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-99F5-4827-9632-6E18FEE23E7A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>power!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>I/O</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>power!$A$2:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7x7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8x8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10x10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>power!$G$2:$G$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-99F5-4827-9632-6E18FEE23E7A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>power!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>XADC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>power!$A$2:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7x7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8x8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10x10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>power!$H$2:$H$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-99F5-4827-9632-6E18FEE23E7A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>power!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PS7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>power!$A$2:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7x7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8x8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10x10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>power!$I$2:$I$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>1.26</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.26</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.26</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.26</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.26</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.26</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-99F5-4827-9632-6E18FEE23E7A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>power!$J$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PL Static</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>power!$A$2:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7x7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8x8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10x10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>power!$J$2:$J$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.13</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-99F5-4827-9632-6E18FEE23E7A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>power!$K$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total Power</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>power!$A$2:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3x3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4x4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5x5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6x6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7x7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8x8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10x10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>power!$K$2:$K$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>1.47</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.47</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.48</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.48</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.49</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.48</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.49</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-99F5-4827-9632-6E18FEE23E7A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:shape val="box"/>
-        <c:axId val="552697656"/>
-        <c:axId val="552698312"/>
-        <c:axId val="359543648"/>
-      </c:bar3DChart>
-      <c:catAx>
-        <c:axId val="552697656"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="552698312"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="552698312"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="552697656"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:serAx>
-        <c:axId val="359543648"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="552698312"/>
-        <c:crosses val="autoZero"/>
-      </c:serAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2817,46 +1604,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3857,500 +2604,6 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4445,47 +2698,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8493DA22-B9A1-40B1-AEA7-E6329094F234}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafico 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57079C7B-B8BF-4C99-84DE-3DB346D139C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4829,7 +3041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9:H9"/>
     </sheetView>
   </sheetViews>
@@ -5158,15 +3370,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -5197,250 +3412,633 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" t="s">
+        <v>6</v>
+      </c>
+      <c r="X1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
-        <v>0.04</v>
-      </c>
-      <c r="C2">
-        <v>0.02</v>
-      </c>
-      <c r="D2">
-        <v>0.01</v>
-      </c>
-      <c r="E2">
-        <v>0.01</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>1.26</v>
-      </c>
-      <c r="J2">
-        <v>0.13</v>
-      </c>
-      <c r="K2">
-        <v>1.47</v>
+      <c r="B2" s="4">
+        <v>3.9190519601106644E-2</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1.5910062938928604E-2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.3120024465024471E-2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>7.6881144195795059E-3</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1.0231699889118318E-5</v>
+      </c>
+      <c r="G2" s="4">
+        <v>2.1401061676442623E-3</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1.9400001037865877E-3</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1.2619483470916748</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0.12661616504192352</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1.4685766696929932</v>
+      </c>
+      <c r="L2">
+        <f>K2-J2-I2</f>
+        <v>8.0012157559394836E-2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="5">
+        <f>B2/L2</f>
+        <v>0.48980705928364243</v>
+      </c>
+      <c r="P2" s="5">
+        <f>C2/L2</f>
+        <v>0.19884556827652353</v>
+      </c>
+      <c r="Q2" s="5">
+        <f>D2/L2</f>
+        <v>0.16397538655653898</v>
+      </c>
+      <c r="R2" s="5">
+        <f>E2/L2</f>
+        <v>9.6086827978266232E-2</v>
+      </c>
+      <c r="S2" s="5">
+        <f>F2/L2</f>
+        <v>1.2787681523927278E-4</v>
+      </c>
+      <c r="T2" s="5">
+        <f>G2/L2</f>
+        <v>2.6747262327673306E-2</v>
+      </c>
+      <c r="U2" s="5">
+        <f>H2/L2</f>
+        <v>2.4246316596905685E-2</v>
+      </c>
+      <c r="W2" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" s="5">
+        <f>I2/K2</f>
+        <v>0.85930028246702694</v>
+      </c>
+      <c r="Y2" s="5">
+        <f>J2/K2</f>
+        <v>8.6216925309315115E-2</v>
+      </c>
+      <c r="Z2" s="5">
+        <f>L2/K2</f>
+        <v>5.4482792223657907E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>0.04</v>
-      </c>
-      <c r="C3">
-        <v>0.02</v>
-      </c>
-      <c r="D3">
-        <v>0.01</v>
-      </c>
-      <c r="E3">
-        <v>0.01</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1.26</v>
-      </c>
-      <c r="J3">
-        <v>0.13</v>
-      </c>
-      <c r="K3">
-        <v>1.47</v>
+      <c r="B3" s="4">
+        <v>4.0350176393985748E-2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.6324156895279884E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.3195060193538666E-2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>9.258653037250042E-3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>5.7229026424465701E-5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>2.2045078221708536E-3</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1.9400001037865877E-3</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1.2619483470916748</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.12773871421813965</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1.4730298519134521</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L8" si="0">K3-J3-I3</f>
+        <v>8.3342790603637695E-2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="5">
+        <f t="shared" ref="O3:O8" si="1">B3/L3</f>
+        <v>0.48414717219973397</v>
+      </c>
+      <c r="P3" s="5">
+        <f t="shared" ref="P3:P8" si="2">C3/L3</f>
+        <v>0.19586765426315564</v>
+      </c>
+      <c r="Q3" s="5">
+        <f t="shared" ref="Q3:Q8" si="3">D3/L3</f>
+        <v>0.15832275470942456</v>
+      </c>
+      <c r="R3" s="5">
+        <f t="shared" ref="R3:R8" si="4">E3/L3</f>
+        <v>0.11109122900962624</v>
+      </c>
+      <c r="S3" s="5">
+        <f t="shared" ref="S3:S8" si="5">F3/L3</f>
+        <v>6.8667038876386996E-4</v>
+      </c>
+      <c r="T3" s="5">
+        <f t="shared" ref="T3:T8" si="6">G3/L3</f>
+        <v>2.6451092004527055E-2</v>
+      </c>
+      <c r="U3" s="5">
+        <f t="shared" ref="U3:U8" si="7">H3/L3</f>
+        <v>2.3277359562062849E-2</v>
+      </c>
+      <c r="W3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X3" s="5">
+        <f t="shared" ref="X3:X8" si="8">I3/K3</f>
+        <v>0.85670249347113747</v>
+      </c>
+      <c r="Y3" s="5">
+        <f t="shared" ref="Y3:Y8" si="9">J3/K3</f>
+        <v>8.6718347256987516E-2</v>
+      </c>
+      <c r="Z3" s="5">
+        <f t="shared" ref="Z3:Z8" si="10">L3/K3</f>
+        <v>5.6579159271875026E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>0.04</v>
-      </c>
-      <c r="C4">
-        <v>0.02</v>
-      </c>
-      <c r="D4">
-        <v>0.01</v>
-      </c>
-      <c r="E4">
-        <v>0.01</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>1.26</v>
-      </c>
-      <c r="J4">
-        <v>0.13</v>
-      </c>
-      <c r="K4">
-        <v>1.48</v>
+      <c r="B4" s="4">
+        <v>4.2696453630924225E-2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.81297417730093E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.3920554891228676E-2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.431964710354805E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.0385630594100803E-4</v>
+      </c>
+      <c r="G4" s="4">
+        <v>3.4746711608022451E-3</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.9400001037865877E-3</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1.2619483470916748</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.12783117592334747</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1.4843775033950806</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>9.4597980380058289E-2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="5">
+        <f t="shared" si="1"/>
+        <v>0.45134635495796316</v>
+      </c>
+      <c r="P4" s="5">
+        <f t="shared" si="2"/>
+        <v>0.19165041050740167</v>
+      </c>
+      <c r="Q4" s="5">
+        <f t="shared" si="3"/>
+        <v>0.14715488465294124</v>
+      </c>
+      <c r="R4" s="5">
+        <f t="shared" si="4"/>
+        <v>0.1513737084662613</v>
+      </c>
+      <c r="S4" s="5">
+        <f t="shared" si="5"/>
+        <v>1.0978702243298784E-3</v>
+      </c>
+      <c r="T4" s="5">
+        <f t="shared" si="6"/>
+        <v>3.6730923290775909E-2</v>
+      </c>
+      <c r="U4" s="5">
+        <f t="shared" si="7"/>
+        <v>2.0507838497105475E-2</v>
+      </c>
+      <c r="W4" t="s">
+        <v>12</v>
+      </c>
+      <c r="X4" s="5">
+        <f t="shared" si="8"/>
+        <v>0.85015324215392385</v>
+      </c>
+      <c r="Y4" s="5">
+        <f t="shared" si="9"/>
+        <v>8.6117699595265315E-2</v>
+      </c>
+      <c r="Z4" s="5">
+        <f t="shared" si="10"/>
+        <v>6.3729058250810863E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
-        <v>0.04</v>
-      </c>
-      <c r="C5">
-        <v>0.02</v>
-      </c>
-      <c r="D5">
-        <v>0.01</v>
-      </c>
-      <c r="E5">
-        <v>0.01</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>1.26</v>
-      </c>
-      <c r="J5">
-        <v>0.13</v>
-      </c>
-      <c r="K5">
-        <v>1.48</v>
+      <c r="B5" s="4">
+        <v>4.2613998055458069E-2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.737813837826252E-2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.3224619440734386E-2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.3507060706615448E-2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2.5030359392985702E-4</v>
+      </c>
+      <c r="G5" s="4">
+        <v>3.0205498915165663E-3</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.9400001037865877E-3</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1.2619483470916748</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.12780939042568207</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1.4817054271697998</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>9.1947689652442932E-2</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="5">
+        <f t="shared" si="1"/>
+        <v>0.46345914961579321</v>
+      </c>
+      <c r="P5" s="5">
+        <f t="shared" si="2"/>
+        <v>0.18900027226296714</v>
+      </c>
+      <c r="Q5" s="5">
+        <f t="shared" si="3"/>
+        <v>0.14382764255113642</v>
+      </c>
+      <c r="R5" s="5">
+        <f t="shared" si="4"/>
+        <v>0.14689940288517714</v>
+      </c>
+      <c r="S5" s="5">
+        <f t="shared" si="5"/>
+        <v>2.7222390782845165E-3</v>
+      </c>
+      <c r="T5" s="5">
+        <f t="shared" si="6"/>
+        <v>3.2850742666118898E-2</v>
+      </c>
+      <c r="U5" s="5">
+        <f t="shared" si="7"/>
+        <v>2.1098954319784199E-2</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X5" s="5">
+        <f t="shared" si="8"/>
+        <v>0.85168639052778383</v>
+      </c>
+      <c r="Y5" s="5">
+        <f t="shared" si="9"/>
+        <v>8.6258299444721825E-2</v>
+      </c>
+      <c r="Z5" s="5">
+        <f t="shared" si="10"/>
+        <v>6.2055310027494384E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
-        <v>0.04</v>
-      </c>
-      <c r="C6">
-        <v>0.02</v>
-      </c>
-      <c r="D6">
-        <v>0.01</v>
-      </c>
-      <c r="E6">
-        <v>0.01</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>1.26</v>
-      </c>
-      <c r="J6">
-        <v>0.13</v>
-      </c>
-      <c r="K6">
-        <v>1.49</v>
+      <c r="B6" s="4">
+        <v>4.4554099440574646E-2</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.981007494032383E-2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.428156066685915E-2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.3419452123343945E-2</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.2719790255650878E-4</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4.4669522903859615E-3</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1.9400001037865877E-3</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1.2619483470916748</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.12786749005317688</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1.488828182220459</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>9.90123450756073E-2</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="5">
+        <f t="shared" si="1"/>
+        <v>0.44998529634413237</v>
+      </c>
+      <c r="P6" s="5">
+        <f t="shared" si="2"/>
+        <v>0.20007681794827262</v>
+      </c>
+      <c r="Q6" s="5">
+        <f t="shared" si="3"/>
+        <v>0.14424020212786132</v>
+      </c>
+      <c r="R6" s="5">
+        <f t="shared" si="4"/>
+        <v>0.13553312077495641</v>
+      </c>
+      <c r="S6" s="5">
+        <f t="shared" si="5"/>
+        <v>5.32456737747129E-3</v>
+      </c>
+      <c r="T6" s="5">
+        <f t="shared" si="6"/>
+        <v>4.5115104454650883E-2</v>
+      </c>
+      <c r="U6" s="5">
+        <f t="shared" si="7"/>
+        <v>1.9593517377102569E-2</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X6" s="5">
+        <f t="shared" si="8"/>
+        <v>0.84761180783775036</v>
+      </c>
+      <c r="Y6" s="5">
+        <f t="shared" si="9"/>
+        <v>8.5884651822263014E-2</v>
+      </c>
+      <c r="Z6" s="5">
+        <f t="shared" si="10"/>
+        <v>6.6503540339986664E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7">
-        <v>0.05</v>
-      </c>
-      <c r="C7">
-        <v>0.02</v>
-      </c>
-      <c r="D7">
-        <v>0.01</v>
-      </c>
-      <c r="E7">
-        <v>0.01</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>1.26</v>
-      </c>
-      <c r="J7">
-        <v>0.13</v>
-      </c>
-      <c r="K7">
-        <v>1.48</v>
+      <c r="B7" s="4">
+        <v>4.6324227005243301E-2</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.9047340378165245E-2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.4235473237931728E-2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>9.6337646245956421E-3</v>
+      </c>
+      <c r="F7" s="4">
+        <v>9.0960034867748618E-5</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2.4676513858139515E-3</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1.9400001037865877E-3</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1.2619483470916748</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.12782421708106995</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1.4835250377655029</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>9.3752473592758179E-2</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.49411205091469257</v>
+      </c>
+      <c r="P7" s="5">
+        <f t="shared" si="2"/>
+        <v>0.20316627016054048</v>
+      </c>
+      <c r="Q7" s="5">
+        <f t="shared" si="3"/>
+        <v>0.15184104154699693</v>
+      </c>
+      <c r="R7" s="5">
+        <f t="shared" si="4"/>
+        <v>0.10275744474159446</v>
+      </c>
+      <c r="S7" s="5">
+        <f t="shared" si="5"/>
+        <v>9.7021477281613547E-4</v>
+      </c>
+      <c r="T7" s="5">
+        <f t="shared" si="6"/>
+        <v>2.6320920304811701E-2</v>
+      </c>
+      <c r="U7" s="5">
+        <f t="shared" si="7"/>
+        <v>2.0692788461385635E-2</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="X7" s="5">
+        <f t="shared" si="8"/>
+        <v>0.85064175862675784</v>
+      </c>
+      <c r="Y7" s="5">
+        <f t="shared" si="9"/>
+        <v>8.61624939432096E-2</v>
+      </c>
+      <c r="Z7" s="5">
+        <f t="shared" si="10"/>
+        <v>6.319574743003252E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8">
-        <v>0.05</v>
-      </c>
-      <c r="C8">
-        <v>0.02</v>
-      </c>
-      <c r="D8">
-        <v>0.01</v>
-      </c>
-      <c r="E8">
-        <v>0.01</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>1.26</v>
-      </c>
-      <c r="J8">
-        <v>0.13</v>
-      </c>
-      <c r="K8">
-        <v>1.49</v>
+      <c r="B8" s="4">
+        <v>4.9014389514923096E-2</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2.120232954621315E-2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.4816205017268658E-2</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.0488901287317276E-2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>8.1412945291958749E-5</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2.7784369885921478E-3</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1.9400001037865877E-3</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1.2619483470916748</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.12787836790084839</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1.4901614189147949</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0.10033470392227173</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="5">
+        <f t="shared" si="1"/>
+        <v>0.48850883691144437</v>
+      </c>
+      <c r="P8" s="5">
+        <f t="shared" si="2"/>
+        <v>0.21131601247997281</v>
+      </c>
+      <c r="Q8" s="5">
+        <f t="shared" si="3"/>
+        <v>0.14766780025330639</v>
+      </c>
+      <c r="R8" s="5">
+        <f t="shared" si="4"/>
+        <v>0.10453911635043964</v>
+      </c>
+      <c r="S8" s="5">
+        <f t="shared" si="5"/>
+        <v>8.1141361970857588E-4</v>
+      </c>
+      <c r="T8" s="5">
+        <f t="shared" si="6"/>
+        <v>2.7691684730983754E-2</v>
+      </c>
+      <c r="U8" s="5">
+        <f t="shared" si="7"/>
+        <v>1.9335285080319627E-2</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X8" s="5">
+        <f t="shared" si="8"/>
+        <v>0.84685345565494807</v>
+      </c>
+      <c r="Y8" s="5">
+        <f t="shared" si="9"/>
+        <v>8.5815111220618898E-2</v>
+      </c>
+      <c r="Z8" s="5">
+        <f t="shared" si="10"/>
+        <v>6.7331433124433016E-2</v>
       </c>
     </row>
     <row r="26" spans="7:7" x14ac:dyDescent="0.3">
@@ -5449,6 +4047,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>